<commit_message>
Updates and Bug Fixes
updated the functionality to make the manual threshold an option for users.

updated the functionality of the file creator to make it add a number to a file if it already exists

fixed a bug where during the merge process I missed a call of the anomaly detection class in the anomaly report function causing it to reset the initial arguments it got fed.
</commit_message>
<xml_diff>
--- a/Data_Cleansing/sasol_data_sample_anomaly_report/xlsx/OXO-5FI696 Augusta_toptagssuboptimal.xlsx
+++ b/Data_Cleansing/sasol_data_sample_anomaly_report/xlsx/OXO-5FI696 Augusta_toptagssuboptimal.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,495 +488,1452 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>43770.04166666666</v>
+        <v>43770</v>
       </c>
       <c r="B2" t="n">
-        <v>9384.63299153646</v>
+        <v>9830.2001953125</v>
       </c>
       <c r="C2" t="n">
-        <v>5950.17383720461</v>
+        <v>5859.125647989908</v>
       </c>
       <c r="D2" t="n">
-        <v>5068.014147949219</v>
+        <v>5069.174365644695</v>
       </c>
       <c r="E2" t="n">
-        <v>9.000414752960205</v>
+        <v>8.99783898188063</v>
       </c>
       <c r="F2" t="n">
-        <v>3095.785913085938</v>
+        <v>2791.424224853517</v>
       </c>
       <c r="G2" t="n">
-        <v>2713.375058513043</v>
+        <v>2710.863008626303</v>
       </c>
       <c r="H2" t="n">
-        <v>132.0638961791992</v>
+        <v>132.091821339505</v>
       </c>
       <c r="I2" t="n">
-        <v>133.9945876177621</v>
+        <v>133.9963000589166</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>43770.08333333334</v>
+        <v>43770.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>9233.277262369793</v>
+        <v>9384.63299153646</v>
       </c>
       <c r="C3" t="n">
-        <v>6379.102249786633</v>
+        <v>5950.17383720461</v>
       </c>
       <c r="D3" t="n">
-        <v>5069.603649902344</v>
+        <v>5068.014147949219</v>
       </c>
       <c r="E3" t="n">
-        <v>8.999083002408346</v>
+        <v>9.000414752960205</v>
       </c>
       <c r="F3" t="n">
-        <v>3201.065022786459</v>
+        <v>3095.785913085938</v>
       </c>
       <c r="G3" t="n">
-        <v>2710.63129272461</v>
+        <v>2713.375058513043</v>
       </c>
       <c r="H3" t="n">
-        <v>132.0354824547007</v>
+        <v>132.0638961791992</v>
       </c>
       <c r="I3" t="n">
-        <v>134.0081062316895</v>
+        <v>133.9945876177621</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>43770.125</v>
+        <v>43770.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>9223.139013671876</v>
+        <v>9233.277262369793</v>
       </c>
       <c r="C4" t="n">
-        <v>6337.343084161932</v>
+        <v>6379.102249786633</v>
       </c>
       <c r="D4" t="n">
-        <v>5061.608939178719</v>
+        <v>5069.603649902344</v>
       </c>
       <c r="E4" t="n">
-        <v>8.997775546709697</v>
+        <v>8.999083002408346</v>
       </c>
       <c r="F4" t="n">
-        <v>3200.161602783204</v>
+        <v>3201.065022786459</v>
       </c>
       <c r="G4" t="n">
-        <v>2710.523927815756</v>
+        <v>2710.63129272461</v>
       </c>
       <c r="H4" t="n">
-        <v>132.0288963317871</v>
+        <v>132.0354824547007</v>
       </c>
       <c r="I4" t="n">
-        <v>134.0083116263398</v>
+        <v>134.0081062316895</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>43770.16666666666</v>
+        <v>43770.125</v>
       </c>
       <c r="B5" t="n">
-        <v>9104.168619791666</v>
+        <v>9223.139013671876</v>
       </c>
       <c r="C5" t="n">
-        <v>6183.590301513672</v>
+        <v>6337.343084161932</v>
       </c>
       <c r="D5" t="n">
-        <v>5004.132636062237</v>
+        <v>5061.608939178719</v>
       </c>
       <c r="E5" t="n">
-        <v>8.998596660296123</v>
+        <v>8.997775546709697</v>
       </c>
       <c r="F5" t="n">
-        <v>3194.761232503256</v>
+        <v>3200.161602783204</v>
       </c>
       <c r="G5" t="n">
-        <v>2719.354256184897</v>
+        <v>2710.523927815756</v>
       </c>
       <c r="H5" t="n">
-        <v>132.0703329291227</v>
+        <v>132.0288963317871</v>
       </c>
       <c r="I5" t="n">
-        <v>134.0020980834962</v>
+        <v>134.0083116263398</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>43771.95833333334</v>
+        <v>43770.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>7975.456363932291</v>
+        <v>9104.168619791666</v>
       </c>
       <c r="C6" t="n">
-        <v>4328.971368408204</v>
+        <v>6183.590301513672</v>
       </c>
       <c r="D6" t="n">
-        <v>4937.812573242188</v>
+        <v>5004.132636062237</v>
       </c>
       <c r="E6" t="n">
-        <v>8.650842966127001</v>
+        <v>8.998596660296123</v>
       </c>
       <c r="F6" t="n">
-        <v>2110.623171997071</v>
+        <v>3194.761232503256</v>
       </c>
       <c r="G6" t="n">
-        <v>1537.311913045248</v>
+        <v>2719.354256184897</v>
       </c>
       <c r="H6" t="n">
-        <v>135.55402247111</v>
+        <v>132.0703329291227</v>
       </c>
       <c r="I6" t="n">
-        <v>136.1321196753132</v>
+        <v>134.0020980834962</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>43772</v>
+        <v>43770.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>8258.268131510416</v>
+        <v>9838.639911042545</v>
       </c>
       <c r="C7" t="n">
-        <v>4904.587259928386</v>
+        <v>6348.371973887211</v>
       </c>
       <c r="D7" t="n">
-        <v>4937.3146705948</v>
+        <v>5004.322265625</v>
       </c>
       <c r="E7" t="n">
-        <v>8.648755582173665</v>
+        <v>8.998671094576517</v>
       </c>
       <c r="F7" t="n">
-        <v>2467.356449381511</v>
+        <v>3100.310658772787</v>
       </c>
       <c r="G7" t="n">
-        <v>1785.101551310222</v>
+        <v>2783.075321451824</v>
       </c>
       <c r="H7" t="n">
-        <v>134.06691269047</v>
+        <v>132.14484565799</v>
       </c>
       <c r="I7" t="n">
-        <v>136.1702276919069</v>
+        <v>134.0009155273438</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>43772.04166666666</v>
+        <v>43770.79166666666</v>
       </c>
       <c r="B8" t="n">
-        <v>8481.239677492253</v>
+        <v>10155.94965457128</v>
       </c>
       <c r="C8" t="n">
-        <v>5041.807727050781</v>
+        <v>6135.916366703254</v>
       </c>
       <c r="D8" t="n">
-        <v>4938.178881835937</v>
+        <v>5068.186745383523</v>
       </c>
       <c r="E8" t="n">
-        <v>8.647890710830689</v>
+        <v>8.950776452777767</v>
       </c>
       <c r="F8" t="n">
-        <v>2503.68212076823</v>
+        <v>2726.429526774089</v>
       </c>
       <c r="G8" t="n">
-        <v>1871.693931070964</v>
+        <v>2559.805867513022</v>
       </c>
       <c r="H8" t="n">
-        <v>135.1884716033936</v>
+        <v>132.0024986267091</v>
       </c>
       <c r="I8" t="n">
-        <v>136.1122201966845</v>
+        <v>134.0131416320801</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>43772.08333333334</v>
+        <v>43770.83333333334</v>
       </c>
       <c r="B9" t="n">
-        <v>8898.724934895834</v>
+        <v>10158.6365641276</v>
       </c>
       <c r="C9" t="n">
-        <v>5056.61567993164</v>
+        <v>6067.128035481771</v>
       </c>
       <c r="D9" t="n">
-        <v>4938.75634765625</v>
+        <v>5068.595555409664</v>
       </c>
       <c r="E9" t="n">
-        <v>8.648796240488688</v>
+        <v>8.944231908183452</v>
       </c>
       <c r="F9" t="n">
-        <v>2446.369386800131</v>
+        <v>2600.456575520834</v>
       </c>
       <c r="G9" t="n">
-        <v>2053.965887451172</v>
+        <v>2561.599346923829</v>
       </c>
       <c r="H9" t="n">
-        <v>135.4231412251792</v>
+        <v>131.9615478515626</v>
       </c>
       <c r="I9" t="n">
-        <v>136.1329421997071</v>
+        <v>134.0034543846836</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>43772.125</v>
+        <v>43770.875</v>
       </c>
       <c r="B10" t="n">
-        <v>8961.214146205357</v>
+        <v>10154.23055826823</v>
       </c>
       <c r="C10" t="n">
-        <v>5009.594675272453</v>
+        <v>6067.04691808364</v>
       </c>
       <c r="D10" t="n">
-        <v>4937.3146705948</v>
+        <v>5068.4115234375</v>
       </c>
       <c r="E10" t="n">
-        <v>8.648107200109658</v>
+        <v>8.952330549558004</v>
       </c>
       <c r="F10" t="n">
-        <v>2350.276317949056</v>
+        <v>2599.769732666016</v>
       </c>
       <c r="G10" t="n">
-        <v>2065.673483455884</v>
+        <v>2566.132640996256</v>
       </c>
       <c r="H10" t="n">
-        <v>135.3992780156498</v>
+        <v>131.9978828430176</v>
       </c>
       <c r="I10" t="n">
-        <v>136.1346825351235</v>
+        <v>134.0003623962403</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>43772.16666666666</v>
+        <v>43770.91666666666</v>
       </c>
       <c r="B11" t="n">
-        <v>8963.184733072916</v>
+        <v>10166.29090983073</v>
       </c>
       <c r="C11" t="n">
-        <v>5187.44690445829</v>
+        <v>5610.986687289782</v>
       </c>
       <c r="D11" t="n">
-        <v>4938.30224609375</v>
+        <v>5069.073815917969</v>
       </c>
       <c r="E11" t="n">
-        <v>8.650172312397602</v>
+        <v>8.95129669413847</v>
       </c>
       <c r="F11" t="n">
-        <v>2333.665065511069</v>
+        <v>2600.405485026043</v>
       </c>
       <c r="G11" t="n">
-        <v>2071.112520345053</v>
+        <v>2565.187208672533</v>
       </c>
       <c r="H11" t="n">
-        <v>135.1721454967152</v>
+        <v>131.9622595009683</v>
       </c>
       <c r="I11" t="n">
-        <v>136.1440934110281</v>
+        <v>134.0040435791016</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>43772.20833333334</v>
+        <v>43770.95833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>8968.128515625</v>
+        <v>10160.84934895833</v>
       </c>
       <c r="C12" t="n">
-        <v>5239.23681233724</v>
+        <v>6105.535599772135</v>
       </c>
       <c r="D12" t="n">
-        <v>4938.191964285715</v>
+        <v>5069.32523163094</v>
       </c>
       <c r="E12" t="n">
-        <v>8.649681973457337</v>
+        <v>8.954678606395879</v>
       </c>
       <c r="F12" t="n">
-        <v>2300.028887939454</v>
+        <v>2599.840649414063</v>
       </c>
       <c r="G12" t="n">
-        <v>2070.785231526693</v>
+        <v>2562.437814759815</v>
       </c>
       <c r="H12" t="n">
-        <v>135.010665124204</v>
+        <v>131.9836158752441</v>
       </c>
       <c r="I12" t="n">
-        <v>136.1479153673189</v>
+        <v>134.0057958177299</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>43772.25</v>
+        <v>43771</v>
       </c>
       <c r="B13" t="n">
-        <v>8971.091667742769</v>
+        <v>10163.93843553046</v>
       </c>
       <c r="C13" t="n">
-        <v>5293.792221966912</v>
+        <v>6080.659326171875</v>
       </c>
       <c r="D13" t="n">
-        <v>4936.98837890625</v>
+        <v>5067.883173581933</v>
       </c>
       <c r="E13" t="n">
-        <v>8.657301775614421</v>
+        <v>8.951937119166056</v>
       </c>
       <c r="F13" t="n">
-        <v>2300.114669421488</v>
+        <v>2610.518383789064</v>
       </c>
       <c r="G13" t="n">
-        <v>2065.219242316633</v>
+        <v>2561.914841715495</v>
       </c>
       <c r="H13" t="n">
-        <v>134.8844699071459</v>
+        <v>131.8745155334474</v>
       </c>
       <c r="I13" t="n">
-        <v>136.149383544922</v>
+        <v>134.0036811828614</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>43772.29166666666</v>
+        <v>43771.91666666666</v>
       </c>
       <c r="B14" t="n">
-        <v>8965.220239257813</v>
+        <v>10161.71319173177</v>
       </c>
       <c r="C14" t="n">
-        <v>5616.239645209194</v>
+        <v>4652.049435450026</v>
       </c>
       <c r="D14" t="n">
-        <v>4938.02978515625</v>
+        <v>5065.754225045196</v>
       </c>
       <c r="E14" t="n">
-        <v>8.661611398061117</v>
+        <v>8.652621285120647</v>
       </c>
       <c r="F14" t="n">
-        <v>2228.390696207683</v>
+        <v>2398.133782958985</v>
       </c>
       <c r="G14" t="n">
-        <v>2058.172786458334</v>
+        <v>2314.175843798425</v>
       </c>
       <c r="H14" t="n">
-        <v>134.8773165149849</v>
+        <v>134.5096738158154</v>
       </c>
       <c r="I14" t="n">
-        <v>136.1496124267579</v>
+        <v>135.737487411499</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>43772.33333333334</v>
+        <v>43771.95833333334</v>
       </c>
       <c r="B15" t="n">
-        <v>8963.406933593749</v>
+        <v>7975.456363932291</v>
       </c>
       <c r="C15" t="n">
-        <v>4819.035675048828</v>
+        <v>4328.971368408204</v>
       </c>
       <c r="D15" t="n">
-        <v>4937.914924172794</v>
+        <v>4937.812573242188</v>
       </c>
       <c r="E15" t="n">
-        <v>8.642122077941895</v>
+        <v>8.650842966127001</v>
       </c>
       <c r="F15" t="n">
-        <v>2178.496803792318</v>
+        <v>2110.623171997071</v>
       </c>
       <c r="G15" t="n">
-        <v>2059.333307346377</v>
+        <v>1537.311913045248</v>
       </c>
       <c r="H15" t="n">
-        <v>134.8263205536141</v>
+        <v>135.55402247111</v>
       </c>
       <c r="I15" t="n">
-        <v>136.1401778292066</v>
+        <v>136.1321196753132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>43772.375</v>
+        <v>43772</v>
       </c>
       <c r="B16" t="n">
-        <v>8958.25586751302</v>
+        <v>8258.268131510416</v>
       </c>
       <c r="C16" t="n">
-        <v>5256.360811121323</v>
+        <v>4904.587259928386</v>
       </c>
       <c r="D16" t="n">
-        <v>4937.904150390625</v>
+        <v>4937.3146705948</v>
       </c>
       <c r="E16" t="n">
-        <v>8.651306287447612</v>
+        <v>8.648755582173665</v>
       </c>
       <c r="F16" t="n">
-        <v>2249.965725938814</v>
+        <v>2467.356449381511</v>
       </c>
       <c r="G16" t="n">
-        <v>2056.693387858073</v>
+        <v>1785.101551310222</v>
       </c>
       <c r="H16" t="n">
-        <v>134.7977973937988</v>
+        <v>134.06691269047</v>
       </c>
       <c r="I16" t="n">
-        <v>136.1428376526392</v>
+        <v>136.1702276919069</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>43772.41666666666</v>
+        <v>43772.04166666666</v>
       </c>
       <c r="B17" t="n">
-        <v>8957.520417542017</v>
+        <v>8481.239677492253</v>
       </c>
       <c r="C17" t="n">
-        <v>5111.833120803202</v>
+        <v>5041.807727050781</v>
       </c>
       <c r="D17" t="n">
-        <v>4938.0751953125</v>
+        <v>4938.178881835937</v>
       </c>
       <c r="E17" t="n">
-        <v>8.657897814114888</v>
+        <v>8.647890710830689</v>
       </c>
       <c r="F17" t="n">
-        <v>2249.89174601237</v>
+        <v>2503.68212076823</v>
       </c>
       <c r="G17" t="n">
-        <v>2053.407336425781</v>
+        <v>1871.693931070964</v>
       </c>
       <c r="H17" t="n">
-        <v>134.6825281778972</v>
+        <v>135.1884716033936</v>
       </c>
       <c r="I17" t="n">
-        <v>136.1508712768555</v>
+        <v>136.1122201966845</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
+        <v>43772.08333333334</v>
+      </c>
+      <c r="B18" t="n">
+        <v>8898.724934895834</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5056.61567993164</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4938.75634765625</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8.648796240488688</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2446.369386800131</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2053.965887451172</v>
+      </c>
+      <c r="H18" t="n">
+        <v>135.4231412251792</v>
+      </c>
+      <c r="I18" t="n">
+        <v>136.1329421997071</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>43772.125</v>
+      </c>
+      <c r="B19" t="n">
+        <v>8961.214146205357</v>
+      </c>
+      <c r="C19" t="n">
+        <v>5009.594675272453</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4937.3146705948</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8.648107200109658</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2350.276317949056</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2065.673483455884</v>
+      </c>
+      <c r="H19" t="n">
+        <v>135.3992780156498</v>
+      </c>
+      <c r="I19" t="n">
+        <v>136.1346825351235</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>43772.16666666666</v>
+      </c>
+      <c r="B20" t="n">
+        <v>8963.184733072916</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5187.44690445829</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4938.30224609375</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8.650172312397602</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2333.665065511069</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2071.112520345053</v>
+      </c>
+      <c r="H20" t="n">
+        <v>135.1721454967152</v>
+      </c>
+      <c r="I20" t="n">
+        <v>136.1440934110281</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>43772.20833333334</v>
+      </c>
+      <c r="B21" t="n">
+        <v>8968.128515625</v>
+      </c>
+      <c r="C21" t="n">
+        <v>5239.23681233724</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4938.191964285715</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8.649681973457337</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2300.028887939454</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2070.785231526693</v>
+      </c>
+      <c r="H21" t="n">
+        <v>135.010665124204</v>
+      </c>
+      <c r="I21" t="n">
+        <v>136.1479153673189</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>43772.25</v>
+      </c>
+      <c r="B22" t="n">
+        <v>8971.091667742769</v>
+      </c>
+      <c r="C22" t="n">
+        <v>5293.792221966912</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4936.98837890625</v>
+      </c>
+      <c r="E22" t="n">
+        <v>8.657301775614421</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2300.114669421488</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2065.219242316633</v>
+      </c>
+      <c r="H22" t="n">
+        <v>134.8844699071459</v>
+      </c>
+      <c r="I22" t="n">
+        <v>136.149383544922</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>43772.29166666666</v>
+      </c>
+      <c r="B23" t="n">
+        <v>8965.220239257813</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5616.239645209194</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4938.02978515625</v>
+      </c>
+      <c r="E23" t="n">
+        <v>8.661611398061117</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2228.390696207683</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2058.172786458334</v>
+      </c>
+      <c r="H23" t="n">
+        <v>134.8773165149849</v>
+      </c>
+      <c r="I23" t="n">
+        <v>136.1496124267579</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>43772.33333333334</v>
+      </c>
+      <c r="B24" t="n">
+        <v>8963.406933593749</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4819.035675048828</v>
+      </c>
+      <c r="D24" t="n">
+        <v>4937.914924172794</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8.642122077941895</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2178.496803792318</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2059.333307346377</v>
+      </c>
+      <c r="H24" t="n">
+        <v>134.8263205536141</v>
+      </c>
+      <c r="I24" t="n">
+        <v>136.1401778292066</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>43772.375</v>
+      </c>
+      <c r="B25" t="n">
+        <v>8958.25586751302</v>
+      </c>
+      <c r="C25" t="n">
+        <v>5256.360811121323</v>
+      </c>
+      <c r="D25" t="n">
+        <v>4937.904150390625</v>
+      </c>
+      <c r="E25" t="n">
+        <v>8.651306287447612</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2249.965725938814</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2056.693387858073</v>
+      </c>
+      <c r="H25" t="n">
+        <v>134.7977973937988</v>
+      </c>
+      <c r="I25" t="n">
+        <v>136.1428376526392</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>43772.41666666666</v>
+      </c>
+      <c r="B26" t="n">
+        <v>8957.520417542017</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5111.833120803202</v>
+      </c>
+      <c r="D26" t="n">
+        <v>4938.0751953125</v>
+      </c>
+      <c r="E26" t="n">
+        <v>8.657897814114888</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2249.89174601237</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2053.407336425781</v>
+      </c>
+      <c r="H26" t="n">
+        <v>134.6825281778972</v>
+      </c>
+      <c r="I26" t="n">
+        <v>136.1508712768555</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
         <v>43772.45833333334</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B27" t="n">
         <v>8965.130657605889</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C27" t="n">
         <v>5275.183653246455</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D27" t="n">
         <v>4937.545537355567</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E27" t="n">
         <v>8.648174293835957</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F27" t="n">
         <v>2330.963421277765</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G27" t="n">
         <v>2057.155013155347</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H27" t="n">
         <v>134.516899814125</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I27" t="n">
         <v>136.1446230549458</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>43772.5</v>
+      </c>
+      <c r="B28" t="n">
+        <v>9530.154354319851</v>
+      </c>
+      <c r="C28" t="n">
+        <v>5446.890556398502</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4937.034167480469</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8.658347296714783</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2479.406545003256</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2304.803381347657</v>
+      </c>
+      <c r="H28" t="n">
+        <v>134.3614895402894</v>
+      </c>
+      <c r="I28" t="n">
+        <v>136.1572991689047</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>43772.54166666666</v>
+      </c>
+      <c r="B29" t="n">
+        <v>9783.172407670454</v>
+      </c>
+      <c r="C29" t="n">
+        <v>5712.773217773438</v>
+      </c>
+      <c r="D29" t="n">
+        <v>4936.759436035156</v>
+      </c>
+      <c r="E29" t="n">
+        <v>8.64757730960846</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2703.42635569853</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2406.1002597328</v>
+      </c>
+      <c r="H29" t="n">
+        <v>134.2838057830555</v>
+      </c>
+      <c r="I29" t="n">
+        <v>136.146434367204</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>43772.58333333334</v>
+      </c>
+      <c r="B30" t="n">
+        <v>9927.526529947916</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5782.940802001953</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4937.217321777343</v>
+      </c>
+      <c r="E30" t="n">
+        <v>8.649336767196655</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2976.961577108084</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2480.602225748699</v>
+      </c>
+      <c r="H30" t="n">
+        <v>134.2254656326672</v>
+      </c>
+      <c r="I30" t="n">
+        <v>136.1477820025988</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>43772.625</v>
+      </c>
+      <c r="B31" t="n">
+        <v>9962.90773535977</v>
+      </c>
+      <c r="C31" t="n">
+        <v>6071.759855895483</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4937.034167480469</v>
+      </c>
+      <c r="E31" t="n">
+        <v>8.648596795667119</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3182.92611287435</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2475.127978112088</v>
+      </c>
+      <c r="H31" t="n">
+        <v>134.2164298947118</v>
+      </c>
+      <c r="I31" t="n">
+        <v>136.13885626272</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>43772.66666666666</v>
+      </c>
+      <c r="B32" t="n">
+        <v>10004.07484826963</v>
+      </c>
+      <c r="C32" t="n">
+        <v>6115.65615234375</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4937.171533203125</v>
+      </c>
+      <c r="E32" t="n">
+        <v>8.644343935753689</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3199.948494466146</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2481.089709472657</v>
+      </c>
+      <c r="H32" t="n">
+        <v>134.1967239379883</v>
+      </c>
+      <c r="I32" t="n">
+        <v>136.1502990722657</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>43772.70833333334</v>
+      </c>
+      <c r="B33" t="n">
+        <v>10046.72832845052</v>
+      </c>
+      <c r="C33" t="n">
+        <v>6056.239738022986</v>
+      </c>
+      <c r="D33" t="n">
+        <v>4937.48486328125</v>
+      </c>
+      <c r="E33" t="n">
+        <v>8.650302646540794</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3050.925423177084</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2482.990470377605</v>
+      </c>
+      <c r="H33" t="n">
+        <v>134.1715278625488</v>
+      </c>
+      <c r="I33" t="n">
+        <v>136.1498413085938</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>43772.75</v>
+      </c>
+      <c r="B34" t="n">
+        <v>10056.75607096354</v>
+      </c>
+      <c r="C34" t="n">
+        <v>5929.296565755209</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4981.143755744485</v>
+      </c>
+      <c r="E34" t="n">
+        <v>8.736200703077079</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3128.396213785808</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2480.98634864102</v>
+      </c>
+      <c r="H34" t="n">
+        <v>134.1552391052246</v>
+      </c>
+      <c r="I34" t="n">
+        <v>136.136527069344</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>43772.79166666666</v>
+      </c>
+      <c r="B35" t="n">
+        <v>10073.43806966146</v>
+      </c>
+      <c r="C35" t="n">
+        <v>5980.169319661459</v>
+      </c>
+      <c r="D35" t="n">
+        <v>5016.992998611829</v>
+      </c>
+      <c r="E35" t="n">
+        <v>8.84656325107863</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3094.050406901042</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2476.734912109376</v>
+      </c>
+      <c r="H35" t="n">
+        <v>134.1886940002442</v>
+      </c>
+      <c r="I35" t="n">
+        <v>136.1531277183726</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>43772.83333333334</v>
+      </c>
+      <c r="B36" t="n">
+        <v>10099.85244954427</v>
+      </c>
+      <c r="C36" t="n">
+        <v>5962.82197265625</v>
+      </c>
+      <c r="D36" t="n">
+        <v>5069.174365644695</v>
+      </c>
+      <c r="E36" t="n">
+        <v>8.851652878375093</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3089.004231770834</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2484.032396048554</v>
+      </c>
+      <c r="H36" t="n">
+        <v>134.1831245422363</v>
+      </c>
+      <c r="I36" t="n">
+        <v>136.1552200317383</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>43772.875</v>
+      </c>
+      <c r="B37" t="n">
+        <v>10156.42995605469</v>
+      </c>
+      <c r="C37" t="n">
+        <v>5972.023659073005</v>
+      </c>
+      <c r="D37" t="n">
+        <v>5069.206274414062</v>
+      </c>
+      <c r="E37" t="n">
+        <v>8.846838267644246</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3099.572989908855</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2548.951444498698</v>
+      </c>
+      <c r="H37" t="n">
+        <v>134.1365089416503</v>
+      </c>
+      <c r="I37" t="n">
+        <v>136.1420593261719</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>43772.91666666666</v>
+      </c>
+      <c r="B38" t="n">
+        <v>10159.99194951418</v>
+      </c>
+      <c r="C38" t="n">
+        <v>6000.826047770182</v>
+      </c>
+      <c r="D38" t="n">
+        <v>5069.382885742188</v>
+      </c>
+      <c r="E38" t="n">
+        <v>8.852490973472595</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3099.878282563026</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2556.658184660584</v>
+      </c>
+      <c r="H38" t="n">
+        <v>134.2049827575684</v>
+      </c>
+      <c r="I38" t="n">
+        <v>136.1428031921387</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>43772.95833333334</v>
+      </c>
+      <c r="B39" t="n">
+        <v>10166.86752647211</v>
+      </c>
+      <c r="C39" t="n">
+        <v>5979.151798973398</v>
+      </c>
+      <c r="D39" t="n">
+        <v>5068.76474609375</v>
+      </c>
+      <c r="E39" t="n">
+        <v>8.859111593550995</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3005.503964763043</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2553.554144741091</v>
+      </c>
+      <c r="H39" t="n">
+        <v>134.1444053649902</v>
+      </c>
+      <c r="I39" t="n">
+        <v>136.1363568266561</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>43773</v>
+      </c>
+      <c r="B40" t="n">
+        <v>10153.77068684896</v>
+      </c>
+      <c r="C40" t="n">
+        <v>5781.218950398763</v>
+      </c>
+      <c r="D40" t="n">
+        <v>5069.106291967975</v>
+      </c>
+      <c r="E40" t="n">
+        <v>8.830073640366232</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2824.26176147461</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2561.618809000652</v>
+      </c>
+      <c r="H40" t="n">
+        <v>134.0866609683706</v>
+      </c>
+      <c r="I40" t="n">
+        <v>135.9725030209839</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>43773.54166666666</v>
+      </c>
+      <c r="B41" t="n">
+        <v>9717.961865637912</v>
+      </c>
+      <c r="C41" t="n">
+        <v>4872.838308113665</v>
+      </c>
+      <c r="D41" t="n">
+        <v>5070.442553710937</v>
+      </c>
+      <c r="E41" t="n">
+        <v>8.846682596206666</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2544.488929239909</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2622.176905103952</v>
+      </c>
+      <c r="H41" t="n">
+        <v>132.7851884206136</v>
+      </c>
+      <c r="I41" t="n">
+        <v>134.0059700012208</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>43773.58333333334</v>
+      </c>
+      <c r="B42" t="n">
+        <v>9844.442473082983</v>
+      </c>
+      <c r="C42" t="n">
+        <v>6569.744838460287</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5023.757397460938</v>
+      </c>
+      <c r="E42" t="n">
+        <v>8.84464385509491</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2906.288092041017</v>
+      </c>
+      <c r="G42" t="n">
+        <v>2640.776108805339</v>
+      </c>
+      <c r="H42" t="n">
+        <v>132.766609064738</v>
+      </c>
+      <c r="I42" t="n">
+        <v>134.0326347351075</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>43773.625</v>
+      </c>
+      <c r="B43" t="n">
+        <v>10169.31243543388</v>
+      </c>
+      <c r="C43" t="n">
+        <v>6020.480114746094</v>
+      </c>
+      <c r="D43" t="n">
+        <v>5005.3212890625</v>
+      </c>
+      <c r="E43" t="n">
+        <v>8.852158482869466</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2971.087375895183</v>
+      </c>
+      <c r="G43" t="n">
+        <v>2814.868115234376</v>
+      </c>
+      <c r="H43" t="n">
+        <v>132.2290126255581</v>
+      </c>
+      <c r="I43" t="n">
+        <v>133.974508994867</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>43773.83333333334</v>
+      </c>
+      <c r="B44" t="n">
+        <v>10039.19246352014</v>
+      </c>
+      <c r="C44" t="n">
+        <v>5933.114473705449</v>
+      </c>
+      <c r="D44" t="n">
+        <v>5004.59930573792</v>
+      </c>
+      <c r="E44" t="n">
+        <v>8.846140154202779</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2864.000952148438</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2714.07021077474</v>
+      </c>
+      <c r="H44" t="n">
+        <v>133.326165008545</v>
+      </c>
+      <c r="I44" t="n">
+        <v>134.6380373636882</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>43773.875</v>
+      </c>
+      <c r="B45" t="n">
+        <v>10062.04959309896</v>
+      </c>
+      <c r="C45" t="n">
+        <v>5910.424890136719</v>
+      </c>
+      <c r="D45" t="n">
+        <v>5005.5029296875</v>
+      </c>
+      <c r="E45" t="n">
+        <v>8.845452904701233</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2802.248303222657</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2717.905568440756</v>
+      </c>
+      <c r="H45" t="n">
+        <v>133.6069526672364</v>
+      </c>
+      <c r="I45" t="n">
+        <v>134.9954130314598</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>43773.91666666666</v>
+      </c>
+      <c r="B46" t="n">
+        <v>10075.26221516927</v>
+      </c>
+      <c r="C46" t="n">
+        <v>6032.192194065126</v>
+      </c>
+      <c r="D46" t="n">
+        <v>5005.892159598215</v>
+      </c>
+      <c r="E46" t="n">
+        <v>8.850423989175749</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2949.197380514706</v>
+      </c>
+      <c r="G46" t="n">
+        <v>2718.084513346354</v>
+      </c>
+      <c r="H46" t="n">
+        <v>133.6089411964101</v>
+      </c>
+      <c r="I46" t="n">
+        <v>134.9856753031412</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>43773.95833333334</v>
+      </c>
+      <c r="B47" t="n">
+        <v>10094.24353841146</v>
+      </c>
+      <c r="C47" t="n">
+        <v>5957.402727111312</v>
+      </c>
+      <c r="D47" t="n">
+        <v>5004.459631347656</v>
+      </c>
+      <c r="E47" t="n">
+        <v>8.851421761512757</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2949.524577495481</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2714.558206353306</v>
+      </c>
+      <c r="H47" t="n">
+        <v>133.6082773929885</v>
+      </c>
+      <c r="I47" t="n">
+        <v>135.0082396189371</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>43774</v>
+      </c>
+      <c r="B48" t="n">
+        <v>10087.56266276042</v>
+      </c>
+      <c r="C48" t="n">
+        <v>5985.0875</v>
+      </c>
+      <c r="D48" t="n">
+        <v>5005.375402832031</v>
+      </c>
+      <c r="E48" t="n">
+        <v>8.842785819371541</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2949.256622314454</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2714.923400878907</v>
+      </c>
+      <c r="H48" t="n">
+        <v>133.6430969238282</v>
+      </c>
+      <c r="I48" t="n">
+        <v>134.9956127166748</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>43774.04166666666</v>
+      </c>
+      <c r="B49" t="n">
+        <v>10084.82131368172</v>
+      </c>
+      <c r="C49" t="n">
+        <v>5924.414177389706</v>
+      </c>
+      <c r="D49" t="n">
+        <v>5004.505419921875</v>
+      </c>
+      <c r="E49" t="n">
+        <v>8.8509601354599</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2813.081118287159</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2717.623526949843</v>
+      </c>
+      <c r="H49" t="n">
+        <v>133.6518898010255</v>
+      </c>
+      <c r="I49" t="n">
+        <v>134.9950279428177</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>43774.08333333334</v>
+      </c>
+      <c r="B50" t="n">
+        <v>10084.86519402118</v>
+      </c>
+      <c r="C50" t="n">
+        <v>5861.537924522211</v>
+      </c>
+      <c r="D50" t="n">
+        <v>5004.368054199219</v>
+      </c>
+      <c r="E50" t="n">
+        <v>8.846257800898275</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2643.197904459636</v>
+      </c>
+      <c r="G50" t="n">
+        <v>2718.125996907553</v>
+      </c>
+      <c r="H50" t="n">
+        <v>133.6561813354492</v>
+      </c>
+      <c r="I50" t="n">
+        <v>135.0029753367105</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>43774.125</v>
+      </c>
+      <c r="B51" t="n">
+        <v>10093.66628643645</v>
+      </c>
+      <c r="C51" t="n">
+        <v>6106.674173990886</v>
+      </c>
+      <c r="D51" t="n">
+        <v>5004.871728515625</v>
+      </c>
+      <c r="E51" t="n">
+        <v>8.852022910118103</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2989.448349125129</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2721.272360052945</v>
+      </c>
+      <c r="H51" t="n">
+        <v>133.6219062805177</v>
+      </c>
+      <c r="I51" t="n">
+        <v>135.0188827514648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>